<commit_message>
Update JS controllers, add validation rules, modify Excel requirements
</commit_message>
<xml_diff>
--- a/docs/FraudShield_requirements.xlsx
+++ b/docs/FraudShield_requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Backend\FraudShield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Backend\FraudShield\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{465EB2B2-3964-4CE3-B4D9-C49E286B0C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CC6FF1-51F2-4E4C-91C3-6CBB98ED0EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,12 +230,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -265,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,10 +299,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,15 +626,15 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="21.75" customWidth="1"/>
-    <col min="4" max="4" width="58.375" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="57.625" customWidth="1"/>
     <col min="5" max="5" width="37.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -800,7 +803,7 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -842,7 +845,7 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="2" t="s">

</xml_diff>